<commit_message>
progress report and testing
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
+++ b/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\W25_4495_S2_ValeriiaN\DocumentsAndReports\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF5D233-9DA3-46C6-8C22-FEB28506AE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E321CE7-2303-466F-AC86-843A087AA6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -330,6 +330,18 @@
   <si>
     <t>Today, I spent time testing the program and improving the structure and functionality across the various pages. I separated the navbar and footer into individual Thymeleaf fragment files to reduce code repetition and successfully connected them to each page using `th:replace`. I also resolved some issues with Bootstrap by ensuring the correct scripts were properly loaded, which fixed the dropdown menu that was not functioning on certain pages. Debugging and testing this took quite a while across different views. As the program expands, it takes more time to test all of its functionality. I have been trying to separate it into different blocks to ensure that changes in one block do not affect the others, but it is not working that way al the time.
 During testing, I encountered a few issues. The "Buyers of My Products" page in the entrepreneur account is not displaying data due to recent changes made in the database schema. I attempted to fix this, but it is still not working as expected. Additionally, I discovered that when a user purchases a product, the product quantity is not updating in the database. This issue needs to be addressed to maintain accurate stock levels.</t>
+  </si>
+  <si>
+    <t>03.04.2025</t>
+  </si>
+  <si>
+    <t>Today, I fixed the buyers' page, which had been crashing due to a change in the database schema. The transaction entity no longer had a direct reference to the product, causing an error in the Thymeleaf template that attempted to access `sale.product.productName`, which no longer existed. To resolve this issue, I updated the page to loop through `transactionProducts` and accessed the product information from there.
+Additionally, I addressed some styling problems on the user registration page. Yesterday, I accidentally removed Bootstrap, but I reintroduced it today and cleaned up the layout.
+Fixed the product qty update after sucesfull purchase.
+Today, I encountered an issue while trying to delete a product. I received a foreign key constraint error because the product was still referenced in the recommendations table as a recommended product. Essentially, Hibernate couldn't delete it since other rows were still pointing to it.
+To resolve this, I realized that I had only mapped the recommendations list for the products that recommend others and not the inverse — the products that are being recommended. So, I added a new list called `recommendedBy` in the Product entity with `mappedBy = "recommendedProduct"` and used `cascade = CascadeType.ALL` along with `orphanRemoval = true`. 
+After making these changes, deleting the product worked perfectly, and all related recommendations were removed automatically.
+Testing the entire thing....</t>
   </si>
 </sst>
 </file>
@@ -668,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +706,7 @@
       </c>
       <c r="G1">
         <f>SUM(B2:B80)</f>
-        <v>78.466999999999999</v>
+        <v>81.466999999999999</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -712,7 +724,7 @@
       </c>
       <c r="G2">
         <f>120-G1</f>
-        <v>41.533000000000001</v>
+        <v>38.533000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1258,10 +1270,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+    <row r="36" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>

</xml_diff>

<commit_message>
request custom amount page fixed
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
+++ b/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\W25_4495_S2_ValeriiaN\DocumentsAndReports\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E321CE7-2303-466F-AC86-843A087AA6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5998C5F5-8CAC-45EA-AF05-05CB4F10AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -342,6 +342,9 @@
 To resolve this, I realized that I had only mapped the recommendations list for the products that recommend others and not the inverse — the products that are being recommended. So, I added a new list called `recommendedBy` in the Product entity with `mappedBy = "recommendedProduct"` and used `cascade = CascadeType.ALL` along with `orphanRemoval = true`. 
 After making these changes, deleting the product worked perfectly, and all related recommendations were removed automatically.
 Testing the entire thing....</t>
+  </si>
+  <si>
+    <t>04.04.2025</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
   <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,7 +1273,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="360" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -1294,9 +1297,17 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>

</xml_diff>

<commit_message>
Final report completion and Presentation
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
+++ b/DocumentsAndReports/Reports/ValeriiaN_Progress_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Desktop\W25_4495_S2_ValeriiaN\DocumentsAndReports\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83437DA-262E-4184-A980-89BA344B29CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4F27F7-36DE-43E2-A3FF-BC5DB9A8A319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="336" windowWidth="17280" windowHeight="10956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -393,6 +393,14 @@
   </si>
   <si>
     <t>Explaining the idea to my basic users and business to collect the feedback</t>
+  </si>
+  <si>
+    <t>11.04.2025</t>
+  </si>
+  <si>
+    <t>Final Report
+Presentation
+Speech Deck</t>
   </si>
 </sst>
 </file>
@@ -731,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +765,7 @@
       </c>
       <c r="G1">
         <f>SUM(B2:B81)</f>
-        <v>89.887</v>
+        <v>93.887</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -775,7 +783,7 @@
       </c>
       <c r="G2">
         <f>120-G1</f>
-        <v>30.113</v>
+        <v>26.113</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1482,10 +1490,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>30</v>
+      </c>
+      <c r="G43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>30</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>

</xml_diff>